<commit_message>
Fix formatting sheet and clean up template sheet
</commit_message>
<xml_diff>
--- a/VBA_Template_2105_andOnwards/TemplateWithoutVBA.xlsx
+++ b/VBA_Template_2105_andOnwards/TemplateWithoutVBA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I529952\Desktop\charts\New Chart files\2105\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E59F62FC-453E-4ED3-833F-4B7CED373CE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B6023E-BAC8-4035-8194-60ADB5295270}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="374" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,6 @@
     <definedName name="SOP_Template_Name">" "</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5914,7 +5913,7 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>1645920</xdr:colOff>
           <xdr:row>108</xdr:row>
-          <xdr:rowOff>83820</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8861,7 +8860,7 @@
           <xdr:col>8</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>60960</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -9234,7 +9233,7 @@
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9438,7 +9437,7 @@
       </c>
       <c r="G11" s="42"/>
       <c r="H11" s="36" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="I11" s="42"/>
       <c r="J11" s="46" t="s">
@@ -13126,7 +13125,7 @@
       <c r="Q1" s="96" t="str">
         <f>"User: "&amp;_xll.IBPUser()&amp;"   |    Planning Area: "&amp;IFERROR(SOP_Planning_Area,"Offline")&amp;"
 "&amp;"Template: "&amp;IFERROR(SOP_Template_Name,"none")</f>
-        <v xml:space="preserve">User: Patrick Weber   |    Planning Area: SAP4PW
+        <v xml:space="preserve">User: #Error, no current connection.   |    Planning Area: SAP4PW
 Template:  </v>
       </c>
       <c r="R1" s="96"/>
@@ -13402,7 +13401,7 @@
       <c r="Q1" s="96" t="str">
         <f>"User: "&amp;_xll.IBPUser()&amp;"   |    Planning Area: "&amp;IFERROR(SOP_Planning_Area,"Offline")&amp;"
 "&amp;"Template: "&amp;IFERROR(SOP_Template_Name,"none")</f>
-        <v xml:space="preserve">User: Patrick Weber   |    Planning Area: SAP4PW
+        <v xml:space="preserve">User: #Error, no current connection.   |    Planning Area: SAP4PW
 Template:  </v>
       </c>
       <c r="R1" s="96"/>

</xml_diff>